<commit_message>
Added method to save combination to cSV file
</commit_message>
<xml_diff>
--- a/src/resources/PythonScripts/excelReaderService/CodeOptions.xlsx
+++ b/src/resources/PythonScripts/excelReaderService/CodeOptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SOFT\JAVA\PartsCodesCombinatorGenerator\src\resources\PythonScripts\excelReaderService\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1714A519-E198-4F64-8639-A06A1BD51F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D135A08-1562-4A12-AD5D-DB42BC874361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="813" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8480" yWindow="-14510" windowWidth="34620" windowHeight="14020" tabRatio="813" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Przewodnik po Numerach" sheetId="12" r:id="rId1"/>
@@ -94,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J71" authorId="0" shapeId="0" xr:uid="{062EAC24-AC7A-43C4-BF87-681E84291EB2}">
+    <comment ref="J71" authorId="0" shapeId="0" xr:uid="{321FF3A1-7D33-426E-B55A-C66258F22E3C}">
       <text>
         <r>
           <rPr>
@@ -108,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J72" authorId="1" shapeId="0" xr:uid="{90E2CFCF-FF83-4FA6-9E5B-1861B935E042}">
+    <comment ref="J72" authorId="1" shapeId="0" xr:uid="{8C8A6013-4FFB-4E67-A999-55B79E02EE10}">
       <text>
         <r>
           <rPr>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="279">
   <si>
     <t>A4</t>
   </si>
@@ -1129,12 +1129,18 @@
   <si>
     <t>Konkatenacja</t>
   </si>
+  <si>
+    <t>Grubosc</t>
+  </si>
+  <si>
+    <t>def.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1276,11 +1282,6 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -1350,7 +1351,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -1680,98 +1681,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="0"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
@@ -1804,62 +1715,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1916,11 +1771,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2075,13 +2047,13 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2093,35 +2065,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2144,30 +2095,6 @@
     <xf numFmtId="49" fontId="0" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2185,37 +2112,31 @@
     <xf numFmtId="49" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2269,11 +2190,490 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="104">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3615,53 +4015,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color rgb="FF000000"/>
@@ -3722,90 +4075,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -3876,88 +4145,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <left style="medium">
           <color rgb="FF000000"/>
@@ -4017,82 +4204,31 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <b/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
+        <sz val="11"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
         <charset val="238"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -4120,188 +4256,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.59999389629810485"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -5082,108 +5036,108 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A31EF3E8-37CA-4B76-8535-B18B9677EC32}" name="Tabela155" displayName="Tabela155" ref="H18:I62" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" tableBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A31EF3E8-37CA-4B76-8535-B18B9677EC32}" name="Tabela155" displayName="Tabela155" ref="H18:I62" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" tableBorderDxfId="69">
   <autoFilter ref="H18:I62" xr:uid="{81B66762-27A3-451B-9D10-170C4497FB19}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E6F300A1-B748-46B0-8F70-9307073EE8B4}" name="Rozmiary Gwintu" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{ADE8550E-B074-47F1-9364-18BB2929E770}" name="Rozmiar gwintu nazw. " dataDxfId="61"/>
+    <tableColumn id="1" xr3:uid="{E6F300A1-B748-46B0-8F70-9307073EE8B4}" name="Rozmiary Gwintu" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{ADE8550E-B074-47F1-9364-18BB2929E770}" name="Rozmiar gwintu nazw. " dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EC3A6DA3-BC7A-4315-8B2E-2E8D3C6DE4B1}" name="Tabela166" displayName="Tabela166" ref="J18:K62" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" tableBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EC3A6DA3-BC7A-4315-8B2E-2E8D3C6DE4B1}" name="Tabela166" displayName="Tabela166" ref="J18:K62" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67" tableBorderDxfId="66">
   <autoFilter ref="J18:K62" xr:uid="{C6AB5C11-06E2-46E0-86C0-4325EB66DBB6}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{63E4A07E-4420-4D51-B9CA-A92F33379DA5}" name="Dlugość gwintu" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{A07B9856-0271-43D0-953B-FF7A8FFD429B}" name="Dla nazwy" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{63E4A07E-4420-4D51-B9CA-A92F33379DA5}" name="Dlugość gwintu" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{A07B9856-0271-43D0-953B-FF7A8FFD429B}" name="Dla nazwy" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{753DCBAA-D245-4265-B3BC-6E4BC412B36B}" name="Tabela187" displayName="Tabela187" ref="L18:L62" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" tableBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{753DCBAA-D245-4265-B3BC-6E4BC412B36B}" name="Tabela187" displayName="Tabela187" ref="L18:L62" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" tableBorderDxfId="63">
   <autoFilter ref="L18:L62" xr:uid="{81F173EC-98D6-48BA-A806-260565541BE6}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{8E129836-4611-46A2-AB86-D6944573D64F}" name="Kolumna1" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{8E129836-4611-46A2-AB86-D6944573D64F}" name="Kolumna1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DBD56F12-08D1-4036-B099-EECFFB308877}" name="Tabela98" displayName="Tabela98" ref="B18:C62" totalsRowShown="0" headerRowDxfId="51" tableBorderDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DBD56F12-08D1-4036-B099-EECFFB308877}" name="Tabela98" displayName="Tabela98" ref="B18:C62" totalsRowShown="0" headerRowDxfId="62" tableBorderDxfId="61">
   <autoFilter ref="B18:C62" xr:uid="{F87B94C2-FCA9-4F2E-AA36-8708BC278EC1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{20CB71AA-C168-49BD-A93F-173B9CF76409}" name="Norma Śrub" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{342EE289-3112-4673-9654-66FE50B51EE1}" name="DIN, ISO" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{20CB71AA-C168-49BD-A93F-173B9CF76409}" name="Norma Śrub" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{342EE289-3112-4673-9654-66FE50B51EE1}" name="DIN, ISO" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D1B111A5-517B-439A-A734-30DEE5E99CDA}" name="Tabela109" displayName="Tabela109" ref="D18:E62" totalsRowShown="0" headerRowDxfId="47" tableBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D1B111A5-517B-439A-A734-30DEE5E99CDA}" name="Tabela109" displayName="Tabela109" ref="D18:E62" totalsRowShown="0" headerRowDxfId="58" tableBorderDxfId="57">
   <autoFilter ref="D18:E62" xr:uid="{D45671F5-1A9D-49A1-A458-ABAA1AB34570}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{BF72DE51-BAF5-4229-88B6-9B1745A47F34}" name="Material" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{54601F66-E844-447C-BD17-BC64E98519C0}" name="material nazw." dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{BF72DE51-BAF5-4229-88B6-9B1745A47F34}" name="Material" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{54601F66-E844-447C-BD17-BC64E98519C0}" name="material nazw." dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{96068E9D-AD60-418B-B72C-B24FE73E1680}" name="Tabela1113" displayName="Tabela1113" ref="F18:G62" totalsRowShown="0" headerRowDxfId="43" tableBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{96068E9D-AD60-418B-B72C-B24FE73E1680}" name="Tabela1113" displayName="Tabela1113" ref="F18:G62" totalsRowShown="0" headerRowDxfId="54" tableBorderDxfId="53">
   <autoFilter ref="F18:G62" xr:uid="{67C209F8-C4B5-422D-AA7F-BCA89B716C6C}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2735FDBF-BA88-491E-8D2F-882666E1B29E}" name="Klasa wytrz." dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{235C42B1-1BE2-4DBF-8467-96BBA51BB8C5}" name="Kolumna1" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{2735FDBF-BA88-491E-8D2F-882666E1B29E}" name="Klasa wytrz." dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{235C42B1-1BE2-4DBF-8467-96BBA51BB8C5}" name="Kolumna1" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{E16F6493-3FFB-437A-ADA3-118E90FCF792}" name="Tabela1514" displayName="Tabela1514" ref="H18:I62" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{E16F6493-3FFB-437A-ADA3-118E90FCF792}" name="Tabela1514" displayName="Tabela1514" ref="H18:I62" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" tableBorderDxfId="48">
   <autoFilter ref="H18:I62" xr:uid="{81B66762-27A3-451B-9D10-170C4497FB19}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FC6836AB-322B-4AC2-9B0F-543409F55F49}" name="Rozmiary Gwintu" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{4A31AD77-5E2D-4E10-AECF-ECB073DA7011}" name="Rozmiar gwintu nazw. " dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{FC6836AB-322B-4AC2-9B0F-543409F55F49}" name="Rozmiary Gwintu" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{4A31AD77-5E2D-4E10-AECF-ECB073DA7011}" name="Rozmiar gwintu nazw. " dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{AB544359-0DF7-44B9-AFB6-F399DA9FEB0A}" name="Tabela1615" displayName="Tabela1615" ref="J18:K62" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" tableBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{AB544359-0DF7-44B9-AFB6-F399DA9FEB0A}" name="Tabela1615" displayName="Tabela1615" ref="J18:K62" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
   <autoFilter ref="J18:K62" xr:uid="{C6AB5C11-06E2-46E0-86C0-4325EB66DBB6}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D77E5097-C92A-4CFD-BA80-CFCA73C15B38}" name="Dlugość gwintu" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{415A04C3-9334-4335-9068-8F0C6E02E38A}" name="Dla nazwy" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{D77E5097-C92A-4CFD-BA80-CFCA73C15B38}" name="Grubosc" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{415A04C3-9334-4335-9068-8F0C6E02E38A}" name="Dla nazwy" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{E889C6A3-7656-4939-8E21-88630F5C2DA9}" name="Tabela1818" displayName="Tabela1818" ref="L18:L62" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{E889C6A3-7656-4939-8E21-88630F5C2DA9}" name="Tabela1818" displayName="Tabela1818" ref="L18:L62" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
   <autoFilter ref="L18:L62" xr:uid="{81F173EC-98D6-48BA-A806-260565541BE6}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B40950C2-923F-472A-88CA-8587D9A5FAA4}" name="Kolumna1" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{B40950C2-923F-472A-88CA-8587D9A5FAA4}" name="Kolumna1" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{3A6ED5F9-F913-421A-8FEE-561B163CD29A}" name="Tabela9220" displayName="Tabela9220" ref="B18:C62" totalsRowShown="0" headerRowDxfId="25" tableBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{3A6ED5F9-F913-421A-8FEE-561B163CD29A}" name="Tabela9220" displayName="Tabela9220" ref="B18:C62" totalsRowShown="0" headerRowDxfId="36" tableBorderDxfId="35">
   <autoFilter ref="B18:C62" xr:uid="{F87B94C2-FCA9-4F2E-AA36-8708BC278EC1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{25638AF6-36B6-4AE3-9EB5-36E730100DD6}" name="Norma Śrub" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{7EB11D70-4A27-435E-96E3-18390F010B82}" name="DIN, ISO" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{25638AF6-36B6-4AE3-9EB5-36E730100DD6}" name="Norma Śrub" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{7EB11D70-4A27-435E-96E3-18390F010B82}" name="DIN, ISO" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5201,54 +5155,54 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{BE63CB27-72CB-49A8-BE5F-B10C0A1DAE15}" name="Tabela10321" displayName="Tabela10321" ref="D18:E62" totalsRowShown="0" headerRowDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{BE63CB27-72CB-49A8-BE5F-B10C0A1DAE15}" name="Tabela10321" displayName="Tabela10321" ref="D18:E62" totalsRowShown="0" headerRowDxfId="32" tableBorderDxfId="31">
   <autoFilter ref="D18:E62" xr:uid="{D45671F5-1A9D-49A1-A458-ABAA1AB34570}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{BB95B611-FC44-4CCD-864E-5B9A3C51D34B}" name="Material" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{5D6C0A73-6C68-47FF-8472-C21E2C32CE48}" name="material nazw." dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{BB95B611-FC44-4CCD-864E-5B9A3C51D34B}" name="Material" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{5D6C0A73-6C68-47FF-8472-C21E2C32CE48}" name="material nazw." dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{962C3CB9-1BF0-42BE-81E1-93B0E90ACCDE}" name="Tabela11422" displayName="Tabela11422" ref="F18:G62" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{962C3CB9-1BF0-42BE-81E1-93B0E90ACCDE}" name="Tabela11422" displayName="Tabela11422" ref="F18:G62" totalsRowShown="0" headerRowDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="F18:G62" xr:uid="{67C209F8-C4B5-422D-AA7F-BCA89B716C6C}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0195BF1B-9887-4D86-9D31-A791AA6826A6}" name="Klasa wytrz." dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{E2F72A83-7EF9-4966-A308-08AE8F836BF4}" name="Kolumna1" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{0195BF1B-9887-4D86-9D31-A791AA6826A6}" name="Klasa wytrz." dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{E2F72A83-7EF9-4966-A308-08AE8F836BF4}" name="Kolumna1" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{7DCE4FA9-B496-4177-B038-A38484CB661A}" name="Tabela15523" displayName="Tabela15523" ref="H18:I62" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{7DCE4FA9-B496-4177-B038-A38484CB661A}" name="Tabela15523" displayName="Tabela15523" ref="H18:I62" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
   <autoFilter ref="H18:I62" xr:uid="{81B66762-27A3-451B-9D10-170C4497FB19}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2A6E1379-C514-48E9-9777-277C89E841F1}" name="Rozmiary Gwintu" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{163C577B-ED5B-4C8B-B02F-43A4F365C783}" name="Rozmiar gwintu nazw. " dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{2A6E1379-C514-48E9-9777-277C89E841F1}" name="Rozmiary Gwintu" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{163C577B-ED5B-4C8B-B02F-43A4F365C783}" name="Rozmiar gwintu nazw. " dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{5D733148-ACD8-4491-B8D8-246361B5D2A8}" name="Tabela16624" displayName="Tabela16624" ref="J18:K62" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{5D733148-ACD8-4491-B8D8-246361B5D2A8}" name="Tabela16624" displayName="Tabela16624" ref="J18:K62" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="J18:K62" xr:uid="{C6AB5C11-06E2-46E0-86C0-4325EB66DBB6}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C5B28BDD-66C2-4433-A7AB-3E595E6A56E3}" name="Dlugość gwintu" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{CAA8F015-19FF-4C30-9EA8-B11A15822E80}" name="Dla nazwy" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{C5B28BDD-66C2-4433-A7AB-3E595E6A56E3}" name="Dlugość gwintu" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{CAA8F015-19FF-4C30-9EA8-B11A15822E80}" name="Dla nazwy" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{5B43B78F-15CE-49B4-A7CA-C8C92AD5241C}" name="Tabela18725" displayName="Tabela18725" ref="L18:L62" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{5B43B78F-15CE-49B4-A7CA-C8C92AD5241C}" name="Tabela18725" displayName="Tabela18725" ref="L18:L62" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="L18:L62" xr:uid="{81F173EC-98D6-48BA-A806-260565541BE6}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{65058BB7-B1E0-46BC-8C82-A920B09CB7E1}" name="Kolumna1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{65058BB7-B1E0-46BC-8C82-A920B09CB7E1}" name="Kolumna1" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5301,30 +5255,30 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3B7865DC-A09D-4F51-A9C9-14A73FF71E5C}" name="Tabela92" displayName="Tabela92" ref="B18:C62" totalsRowShown="0" headerRowDxfId="77" tableBorderDxfId="76">
   <autoFilter ref="B18:C62" xr:uid="{F87B94C2-FCA9-4F2E-AA36-8708BC278EC1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C893B547-5B39-4A89-A329-3C4FF2E6F571}" name="Norma Śrub" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{3444D0ED-7FBD-4344-82C2-0EC67FDDCB4D}" name="DIN, ISO" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{C893B547-5B39-4A89-A329-3C4FF2E6F571}" name="Norma Śrub" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{3444D0ED-7FBD-4344-82C2-0EC67FDDCB4D}" name="DIN, ISO" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ECC2F9B0-0FB9-46BF-9C47-684B9333B034}" name="Tabela103" displayName="Tabela103" ref="D18:E62" totalsRowShown="0" headerRowDxfId="73" tableBorderDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ECC2F9B0-0FB9-46BF-9C47-684B9333B034}" name="Tabela103" displayName="Tabela103" ref="D18:E62" totalsRowShown="0" headerRowDxfId="75" tableBorderDxfId="74">
   <autoFilter ref="D18:E62" xr:uid="{D45671F5-1A9D-49A1-A458-ABAA1AB34570}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{610FFA75-AC9F-451C-B082-A734A2030FD2}" name="Material" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{0FE9965B-E3E9-4F6D-A9BC-140D8814507C}" name="material nazw." dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{610FFA75-AC9F-451C-B082-A734A2030FD2}" name="Material" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{0FE9965B-E3E9-4F6D-A9BC-140D8814507C}" name="material nazw." dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6846552F-4B37-4B52-879D-839938BE0DD2}" name="Tabela114" displayName="Tabela114" ref="F18:G62" totalsRowShown="0" headerRowDxfId="69" tableBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6846552F-4B37-4B52-879D-839938BE0DD2}" name="Tabela114" displayName="Tabela114" ref="F18:G62" totalsRowShown="0" headerRowDxfId="73" tableBorderDxfId="72">
   <autoFilter ref="F18:G62" xr:uid="{67C209F8-C4B5-422D-AA7F-BCA89B716C6C}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0742B3C3-1491-4AF6-8F55-71F1703C4709}" name="Klasa wytrz." dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{743D2D5F-29C0-430C-B3DB-A47F9506D7DB}" name="Kolumna1" dataDxfId="66"/>
+    <tableColumn id="1" xr3:uid="{0742B3C3-1491-4AF6-8F55-71F1703C4709}" name="Klasa wytrz." dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{743D2D5F-29C0-430C-B3DB-A47F9506D7DB}" name="Kolumna1" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5651,7 +5605,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17.649999999999999" x14ac:dyDescent="0.5">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="71" t="s">
         <v>222</v>
       </c>
     </row>
@@ -5694,7 +5648,7 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="66" t="s">
         <v>176</v>
       </c>
       <c r="B9" s="2"/>
@@ -5706,7 +5660,7 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="20.55" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="76" t="s">
+      <c r="A10" s="67" t="s">
         <v>223</v>
       </c>
       <c r="B10" s="2"/>
@@ -5718,7 +5672,7 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="68" t="s">
         <v>199</v>
       </c>
       <c r="B11" s="2"/>
@@ -5730,7 +5684,7 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="69" t="s">
         <v>179</v>
       </c>
       <c r="B12" s="2"/>
@@ -5742,7 +5696,7 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="70" t="s">
         <v>221</v>
       </c>
       <c r="B13" s="2"/>
@@ -5760,14 +5714,14 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="117" t="s">
+      <c r="A16" s="98" t="s">
         <v>261</v>
       </c>
-      <c r="B16" s="117"/>
-      <c r="C16" s="117"/>
-      <c r="D16" s="117"/>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
     </row>
     <row r="17" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -5825,7 +5779,7 @@
       <c r="D26" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="R26" s="81"/>
+      <c r="R26" s="72"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="R28" s="32"/>
@@ -5842,23 +5796,23 @@
       <c r="B30" t="s">
         <v>268</v>
       </c>
-      <c r="D30" s="117"/>
-      <c r="E30" s="117"/>
-      <c r="F30" s="117"/>
-      <c r="G30" s="117"/>
-      <c r="H30" s="117"/>
-      <c r="I30" s="117"/>
-      <c r="J30" s="117"/>
-      <c r="K30" s="117"/>
-      <c r="L30" s="117"/>
-      <c r="M30" s="117"/>
-      <c r="N30" s="117"/>
-      <c r="O30" s="117"/>
-      <c r="P30" s="117"/>
-      <c r="Q30" s="117"/>
-      <c r="R30" s="117"/>
-      <c r="S30" s="117"/>
-      <c r="T30" s="117"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="98"/>
+      <c r="F30" s="98"/>
+      <c r="G30" s="98"/>
+      <c r="H30" s="98"/>
+      <c r="I30" s="98"/>
+      <c r="J30" s="98"/>
+      <c r="K30" s="98"/>
+      <c r="L30" s="98"/>
+      <c r="M30" s="98"/>
+      <c r="N30" s="98"/>
+      <c r="O30" s="98"/>
+      <c r="P30" s="98"/>
+      <c r="Q30" s="98"/>
+      <c r="R30" s="98"/>
+      <c r="S30" s="98"/>
+      <c r="T30" s="98"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
@@ -5931,10 +5885,10 @@
   <sheetPr codeName="Arkusz3">
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AD76"/>
+  <dimension ref="A1:AD73"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -5962,11 +5916,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="99" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
       <c r="D1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -6053,7 +6007,7 @@
       </c>
       <c r="G7" s="41" t="str">
         <f>VLOOKUP($G$6,Tabela11[],2,0)</f>
-        <v xml:space="preserve"> </v>
+        <v>-</v>
       </c>
       <c r="H7" s="38" t="s">
         <v>113</v>
@@ -6091,20 +6045,20 @@
         <f>_xlfn.CONCAT(C6:K6)</f>
         <v>00912-A00-F48-008</v>
       </c>
-      <c r="D9" s="119" t="str">
+      <c r="D9" s="100" t="str">
         <f>_xlfn.CONCAT(C7:L7)</f>
-        <v xml:space="preserve">DIN 912 Śruba walc. imbus Alu.   fi4,8 x8 </v>
-      </c>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="120"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="121"/>
-      <c r="K9" s="124" t="s">
+        <v xml:space="preserve">DIN 912 Śruba walc. imbus Alu. - fi4,8 x8 </v>
+      </c>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="105" t="s">
         <v>186</v>
       </c>
-      <c r="L9" s="125"/>
+      <c r="L9" s="106"/>
       <c r="M9" s="4">
         <f>LEN(C9)</f>
         <v>17</v>
@@ -6125,20 +6079,20 @@
         <f>_xlfn.CONCAT(C6:M6)</f>
         <v>00912-A00-F48-008-00</v>
       </c>
-      <c r="D10" s="119" t="str">
+      <c r="D10" s="100" t="str">
         <f>_xlfn.CONCAT(C7:M7)</f>
-        <v xml:space="preserve">DIN 912 Śruba walc. imbus Alu.   fi4,8 x8 </v>
-      </c>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="120"/>
-      <c r="I10" s="120"/>
-      <c r="J10" s="121"/>
-      <c r="K10" s="122" t="s">
+        <v xml:space="preserve">DIN 912 Śruba walc. imbus Alu. - fi4,8 x8 </v>
+      </c>
+      <c r="E10" s="101"/>
+      <c r="F10" s="101"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="101"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="103" t="s">
         <v>185</v>
       </c>
-      <c r="L10" s="123"/>
+      <c r="L10" s="104"/>
       <c r="M10" s="4">
         <f>LEN(C10)</f>
         <v>20</v>
@@ -6329,7 +6283,7 @@
       <c r="B19" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="71" t="s">
+      <c r="C19" s="64" t="s">
         <v>214</v>
       </c>
       <c r="D19" s="15" t="s">
@@ -6342,7 +6296,7 @@
         <v>19</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="H19" s="54" t="s">
         <v>36</v>
@@ -6378,7 +6332,7 @@
       <c r="B20" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="72" t="s">
+      <c r="C20" s="65" t="s">
         <v>213</v>
       </c>
       <c r="D20" s="16" t="s">
@@ -6476,7 +6430,7 @@
       <c r="B22" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="65" t="s">
         <v>211</v>
       </c>
       <c r="D22" s="16" t="s">
@@ -6795,10 +6749,10 @@
       <c r="Y29" s="2"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B30" s="82" t="s">
+      <c r="B30" s="73" t="s">
         <v>226</v>
       </c>
-      <c r="C30" s="83" t="s">
+      <c r="C30" s="74" t="s">
         <v>241</v>
       </c>
       <c r="D30" s="16"/>
@@ -7064,10 +7018,10 @@
       <c r="E39" s="21"/>
       <c r="F39" s="16"/>
       <c r="G39" s="10"/>
-      <c r="H39" s="84" t="s">
+      <c r="H39" s="75" t="s">
         <v>234</v>
       </c>
-      <c r="I39" s="85" t="s">
+      <c r="I39" s="76" t="s">
         <v>230</v>
       </c>
       <c r="J39" s="54" t="s">
@@ -7088,10 +7042,10 @@
       <c r="E40" s="21"/>
       <c r="F40" s="16"/>
       <c r="G40" s="10"/>
-      <c r="H40" s="84" t="s">
+      <c r="H40" s="75" t="s">
         <v>235</v>
       </c>
-      <c r="I40" s="85" t="s">
+      <c r="I40" s="76" t="s">
         <v>229</v>
       </c>
       <c r="J40" s="54" t="s">
@@ -7112,10 +7066,10 @@
       <c r="E41" s="21"/>
       <c r="F41" s="16"/>
       <c r="G41" s="10"/>
-      <c r="H41" s="84" t="s">
+      <c r="H41" s="75" t="s">
         <v>236</v>
       </c>
-      <c r="I41" s="85" t="s">
+      <c r="I41" s="76" t="s">
         <v>227</v>
       </c>
       <c r="J41" s="54" t="s">
@@ -7136,10 +7090,10 @@
       <c r="E42" s="21"/>
       <c r="F42" s="16"/>
       <c r="G42" s="10"/>
-      <c r="H42" s="84" t="s">
+      <c r="H42" s="75" t="s">
         <v>237</v>
       </c>
-      <c r="I42" s="85" t="s">
+      <c r="I42" s="76" t="s">
         <v>231</v>
       </c>
       <c r="J42" s="54" t="s">
@@ -7160,10 +7114,10 @@
       <c r="E43" s="21"/>
       <c r="F43" s="16"/>
       <c r="G43" s="10"/>
-      <c r="H43" s="84" t="s">
+      <c r="H43" s="75" t="s">
         <v>238</v>
       </c>
-      <c r="I43" s="85" t="s">
+      <c r="I43" s="76" t="s">
         <v>232</v>
       </c>
       <c r="J43" s="54" t="s">
@@ -7184,10 +7138,10 @@
       <c r="E44" s="21"/>
       <c r="F44" s="16"/>
       <c r="G44" s="10"/>
-      <c r="H44" s="84" t="s">
+      <c r="H44" s="75" t="s">
         <v>239</v>
       </c>
-      <c r="I44" s="85" t="s">
+      <c r="I44" s="76" t="s">
         <v>233</v>
       </c>
       <c r="J44" s="54" t="s">
@@ -7208,10 +7162,10 @@
       <c r="E45" s="21"/>
       <c r="F45" s="16"/>
       <c r="G45" s="10"/>
-      <c r="H45" s="84" t="s">
+      <c r="H45" s="75" t="s">
         <v>240</v>
       </c>
-      <c r="I45" s="85" t="s">
+      <c r="I45" s="76" t="s">
         <v>228</v>
       </c>
       <c r="J45" s="54" t="s">
@@ -7527,158 +7481,120 @@
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B70" s="63" t="s">
+      <c r="B70" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="73"/>
-      <c r="D70" s="87" t="s">
+      <c r="C70" s="64" t="s">
+        <v>214</v>
+      </c>
+      <c r="D70" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E70" s="67"/>
-      <c r="F70" s="87" t="s">
+      <c r="E70" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F70" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G70" s="89"/>
-      <c r="H70" s="65" t="s">
-        <v>36</v>
-      </c>
-      <c r="I70" s="70"/>
-      <c r="J70" s="65" t="s">
-        <v>271</v>
-      </c>
-      <c r="K70" s="69"/>
+      <c r="G70" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="H70" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="I70" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="J70" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="K70" s="63" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B71" s="62" t="s">
+      <c r="B71" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C71" s="74"/>
-      <c r="D71" s="88" t="s">
+      <c r="C71" s="65" t="s">
+        <v>213</v>
+      </c>
+      <c r="D71" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E71" s="68"/>
-      <c r="F71" s="88" t="s">
+      <c r="E71" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F71" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G71" s="90"/>
-      <c r="H71" s="65" t="s">
-        <v>38</v>
-      </c>
-      <c r="I71" s="70"/>
-      <c r="J71" s="65" t="s">
-        <v>242</v>
-      </c>
-      <c r="K71" s="70"/>
+      <c r="G71" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H71" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="I71" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="J71" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="K71" s="63" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B72" s="64" t="s">
+      <c r="B72" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="C72" s="66"/>
-      <c r="D72" s="88" t="s">
-        <v>13</v>
-      </c>
-      <c r="E72" s="68"/>
-      <c r="F72" s="88">
+      <c r="C72" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="D72" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E72" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="F72" s="16">
         <v>80</v>
       </c>
-      <c r="G72" s="90"/>
-      <c r="H72" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="I72" s="70"/>
-      <c r="J72" s="65" t="s">
-        <v>25</v>
-      </c>
-      <c r="K72" s="70"/>
+      <c r="G72" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H72" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="I72" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="J72" s="62" t="s">
+        <v>30</v>
+      </c>
+      <c r="K72" s="63" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B73" s="64" t="s">
+      <c r="B73" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C73" s="74"/>
-      <c r="D73" s="88" t="s">
-        <v>14</v>
-      </c>
-      <c r="E73" s="68"/>
-      <c r="F73" s="88" t="s">
+      <c r="C73" s="65" t="s">
+        <v>211</v>
+      </c>
+      <c r="D73" s="16"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G73" s="90"/>
-      <c r="H73" s="65" t="s">
-        <v>44</v>
-      </c>
-      <c r="I73" s="70"/>
-      <c r="J73" s="65" t="s">
-        <v>26</v>
-      </c>
-      <c r="K73" s="70"/>
-    </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B74" s="64" t="s">
-        <v>200</v>
-      </c>
-      <c r="C74" s="66"/>
-      <c r="D74" s="88" t="s">
-        <v>15</v>
-      </c>
-      <c r="E74" s="68"/>
-      <c r="F74" s="88" t="s">
-        <v>18</v>
-      </c>
-      <c r="G74" s="90"/>
-      <c r="H74" s="65" t="s">
-        <v>22</v>
-      </c>
-      <c r="I74" s="70"/>
-      <c r="J74" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="K74" s="70"/>
-    </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B75" s="62" t="s">
-        <v>90</v>
-      </c>
-      <c r="C75" s="66"/>
-      <c r="D75" s="88" t="s">
-        <v>152</v>
-      </c>
-      <c r="E75" s="68"/>
-      <c r="F75" s="88" t="s">
-        <v>181</v>
-      </c>
-      <c r="G75" s="90"/>
-      <c r="H75" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="I75" s="70"/>
-      <c r="J75" s="65" t="s">
-        <v>28</v>
-      </c>
-      <c r="K75" s="70"/>
-    </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B76" s="64" t="s">
-        <v>91</v>
-      </c>
-      <c r="C76" s="66"/>
-      <c r="D76" s="88" t="s">
-        <v>224</v>
-      </c>
-      <c r="E76" s="68"/>
-      <c r="F76" s="88" t="s">
-        <v>182</v>
-      </c>
-      <c r="G76" s="90"/>
-      <c r="H76" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="I76" s="70"/>
-      <c r="J76" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="K76" s="70"/>
+      <c r="G73" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="H73" s="54"/>
+      <c r="I73" s="11"/>
+      <c r="J73" s="54"/>
+      <c r="K73" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -7734,17 +7650,17 @@
   <sheetPr codeName="Arkusz4">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AD73"/>
+  <dimension ref="A1:AD72"/>
   <sheetViews>
-    <sheetView topLeftCell="B36" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69:K73"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.265625" customWidth="1"/>
     <col min="2" max="2" width="16.9296875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="35.73046875" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="14.59765625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
@@ -7765,11 +7681,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="99" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
       <c r="D1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -7856,7 +7772,7 @@
       </c>
       <c r="G7" s="41" t="str">
         <f>VLOOKUP($G$6,Tabela114[],2,0)</f>
-        <v xml:space="preserve"> </v>
+        <v>-</v>
       </c>
       <c r="H7" s="38" t="s">
         <v>113</v>
@@ -7889,20 +7805,20 @@
         <f>_xlfn.CONCAT(C6:K6)</f>
         <v>00315-N00-100-001</v>
       </c>
-      <c r="D9" s="119" t="str">
+      <c r="D9" s="100" t="str">
         <f>_xlfn.CONCAT(C7:L7)</f>
-        <v xml:space="preserve">DIN 315 Nakrętka motylkowa A2   M10 </v>
-      </c>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="120"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="121"/>
-      <c r="K9" s="124" t="s">
+        <v xml:space="preserve">DIN 315 Nakrętka motylkowa A2 - M10 </v>
+      </c>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="105" t="s">
         <v>186</v>
       </c>
-      <c r="L9" s="125"/>
+      <c r="L9" s="106"/>
       <c r="N9" s="4">
         <f>LEN(D9)</f>
         <v>36</v>
@@ -7919,20 +7835,20 @@
         <f>_xlfn.CONCAT(C6:M6)</f>
         <v>00315-N00-100-001-00</v>
       </c>
-      <c r="D10" s="119" t="str">
+      <c r="D10" s="100" t="str">
         <f>_xlfn.CONCAT(C7:M7)</f>
-        <v xml:space="preserve">DIN 315 Nakrętka motylkowa A2   M10 </v>
-      </c>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="120"/>
-      <c r="I10" s="120"/>
-      <c r="J10" s="121"/>
-      <c r="K10" s="122" t="s">
+        <v xml:space="preserve">DIN 315 Nakrętka motylkowa A2 - M10 </v>
+      </c>
+      <c r="E10" s="101"/>
+      <c r="F10" s="101"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="101"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="103" t="s">
         <v>185</v>
       </c>
-      <c r="L10" s="123"/>
+      <c r="L10" s="104"/>
       <c r="N10" s="4">
         <f>LEN(D10)</f>
         <v>36</v>
@@ -8114,11 +8030,11 @@
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
     </row>
-    <row r="19" spans="2:27" ht="13.15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B19" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="111" t="s">
         <v>216</v>
       </c>
       <c r="D19" s="15" t="s">
@@ -8131,20 +8047,22 @@
         <v>19</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="H19" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="J19" s="60" t="s">
+      <c r="J19" s="113" t="s">
         <v>80</v>
       </c>
-      <c r="K19" s="17"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="56" t="s">
+      <c r="K19" s="114" t="s">
+        <v>81</v>
+      </c>
+      <c r="L19" s="112"/>
+      <c r="M19" s="115" t="s">
         <v>19</v>
       </c>
       <c r="O19" s="3"/>
@@ -9123,17 +9041,17 @@
       <c r="M61" s="57"/>
     </row>
     <row r="62" spans="2:25" ht="49.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="13"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="21"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="10"/>
-      <c r="H62" s="54"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="54"/>
-      <c r="K62" s="11"/>
-      <c r="L62" s="54"/>
+      <c r="B62" s="116"/>
+      <c r="C62" s="117"/>
+      <c r="D62" s="118"/>
+      <c r="E62" s="117"/>
+      <c r="F62" s="118"/>
+      <c r="G62" s="119"/>
+      <c r="H62" s="120"/>
+      <c r="I62" s="121"/>
+      <c r="J62" s="120"/>
+      <c r="K62" s="121"/>
+      <c r="L62" s="120"/>
       <c r="M62" s="58"/>
     </row>
     <row r="69" spans="2:11" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
@@ -9141,87 +9059,101 @@
         <v>276</v>
       </c>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B70" s="91" t="s">
+    <row r="70" spans="2:11" ht="13.15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="C70" s="73"/>
-      <c r="D70" s="87" t="s">
+      <c r="C70" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="D70" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E70" s="67"/>
-      <c r="F70" s="87" t="s">
+      <c r="E70" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F70" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G70" s="89"/>
-      <c r="H70" s="94" t="s">
+      <c r="G70" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="H70" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="I70" s="70"/>
-      <c r="J70" s="94" t="s">
+      <c r="I70" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="J70" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="K70" s="69"/>
+      <c r="K70" s="17" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B71" s="92" t="s">
+      <c r="B71" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C71" s="74"/>
-      <c r="D71" s="88" t="s">
+      <c r="C71" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="D71" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E71" s="68"/>
-      <c r="F71" s="88" t="s">
+      <c r="E71" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F71" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G71" s="90"/>
-      <c r="H71" s="94" t="s">
+      <c r="G71" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H71" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="I71" s="70"/>
-      <c r="J71" s="94" t="s">
+      <c r="I71" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J71" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="K71" s="70"/>
+      <c r="K71" s="18" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B72" s="93" t="s">
+      <c r="B72" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="C72" s="66"/>
-      <c r="D72" s="88" t="s">
+      <c r="C72" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="D72" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E72" s="68"/>
-      <c r="F72" s="88">
+      <c r="E72" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="F72" s="16">
         <v>80</v>
       </c>
-      <c r="G72" s="90"/>
-      <c r="H72" s="94" t="s">
+      <c r="G72" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H72" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="I72" s="70"/>
-      <c r="J72" s="94" t="s">
+      <c r="I72" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J72" s="60" t="s">
         <v>82</v>
       </c>
-      <c r="K72" s="70"/>
-    </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B73" s="92" t="s">
-        <v>71</v>
-      </c>
-      <c r="C73" s="74"/>
-      <c r="D73" s="88"/>
-      <c r="E73" s="68"/>
-      <c r="F73" s="88"/>
-      <c r="G73" s="90"/>
-      <c r="H73" s="94" t="s">
-        <v>44</v>
-      </c>
-      <c r="I73" s="70"/>
-      <c r="J73" s="65"/>
-      <c r="K73" s="70"/>
+      <c r="K72" s="18" t="s">
+        <v>141</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -9231,7 +9163,7 @@
     <mergeCell ref="D10:J10"/>
     <mergeCell ref="K10:L10"/>
   </mergeCells>
-  <dataValidations count="7">
+  <dataValidations disablePrompts="1" count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{4FEF0FAC-0422-486C-875A-BA1774E72A47}">
       <formula1>$B$19:$B$61</formula1>
     </dataValidation>
@@ -9276,10 +9208,10 @@
   <sheetPr codeName="Arkusz5">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AD74"/>
+  <dimension ref="A1:AD72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -9293,8 +9225,7 @@
     <col min="7" max="7" width="13.59765625" style="4" customWidth="1"/>
     <col min="8" max="8" width="21.1328125" style="4" customWidth="1"/>
     <col min="9" max="9" width="24.73046875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="13.9296875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="10.59765625" style="4" customWidth="1"/>
+    <col min="10" max="11" width="19.59765625" style="4" customWidth="1"/>
     <col min="12" max="12" width="15.59765625" style="4" customWidth="1"/>
     <col min="13" max="13" width="16.73046875" style="4" customWidth="1"/>
     <col min="14" max="14" width="8.86328125" style="4" customWidth="1"/>
@@ -9307,11 +9238,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="99" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
       <c r="D1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -9382,37 +9313,37 @@
       <c r="B7" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="113" t="str">
+      <c r="C7" s="94" t="str">
         <f>VLOOKUP($C$6,Tabela98[],2,0)</f>
         <v>DIN 440 Podkladka Poszerzana 2x</v>
       </c>
-      <c r="D7" s="113" t="s">
+      <c r="D7" s="94" t="s">
         <v>113</v>
       </c>
-      <c r="E7" s="113" t="str">
+      <c r="E7" s="94" t="str">
         <f>VLOOKUP($E$6,Tabela109[],2,0)</f>
         <v>Ocynk</v>
       </c>
-      <c r="F7" s="113" t="s">
+      <c r="F7" s="94" t="s">
         <v>113</v>
       </c>
-      <c r="G7" s="113" t="str">
+      <c r="G7" s="94" t="str">
         <f>VLOOKUP($G$6,Tabela1113[],2,0)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H7" s="113" t="s">
+        <v>-</v>
+      </c>
+      <c r="H7" s="94" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="113" t="str">
+      <c r="I7" s="94" t="str">
         <f>VLOOKUP($I$6,Tabela1514[],2,0)</f>
         <v>M14</v>
       </c>
-      <c r="J7" s="113"/>
-      <c r="K7" s="114"/>
-      <c r="L7" s="115" t="s">
+      <c r="J7" s="94"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="96" t="s">
         <v>113</v>
       </c>
-      <c r="M7" s="116"/>
+      <c r="M7" s="97"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
@@ -9431,20 +9362,20 @@
         <f>_xlfn.CONCAT(C6:K6)</f>
         <v>00440-O00-140-001</v>
       </c>
-      <c r="D9" s="119" t="str">
+      <c r="D9" s="100" t="str">
         <f>_xlfn.CONCAT(C7:L7)</f>
-        <v xml:space="preserve">DIN 440 Podkladka Poszerzana 2x Ocynk   M14 </v>
-      </c>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="120"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="121"/>
-      <c r="K9" s="126" t="s">
+        <v xml:space="preserve">DIN 440 Podkladka Poszerzana 2x Ocynk - M14 </v>
+      </c>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="107" t="s">
         <v>186</v>
       </c>
-      <c r="L9" s="127"/>
+      <c r="L9" s="108"/>
       <c r="N9" s="4">
         <f>LEN(D9)</f>
         <v>44</v>
@@ -9461,20 +9392,20 @@
         <f>_xlfn.CONCAT(C6:M6)</f>
         <v>00440-O00-140-001-00</v>
       </c>
-      <c r="D10" s="119" t="str">
+      <c r="D10" s="100" t="str">
         <f>_xlfn.CONCAT(C7:M7)</f>
-        <v xml:space="preserve">DIN 440 Podkladka Poszerzana 2x Ocynk   M14 </v>
-      </c>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="120"/>
-      <c r="I10" s="120"/>
-      <c r="J10" s="121"/>
-      <c r="K10" s="128" t="s">
+        <v xml:space="preserve">DIN 440 Podkladka Poszerzana 2x Ocynk - M14 </v>
+      </c>
+      <c r="E10" s="101"/>
+      <c r="F10" s="101"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="101"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="109" t="s">
         <v>185</v>
       </c>
-      <c r="L10" s="129"/>
+      <c r="L10" s="110"/>
       <c r="N10" s="4">
         <f>LEN(D10)</f>
         <v>44</v>
@@ -9609,40 +9540,40 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="2:27" ht="17.55" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="103" t="s">
+      <c r="B18" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="104" t="s">
+      <c r="C18" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="104" t="s">
+      <c r="D18" s="86" t="s">
         <v>93</v>
       </c>
-      <c r="E18" s="103" t="s">
+      <c r="E18" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="F18" s="104" t="s">
+      <c r="F18" s="86" t="s">
         <v>184</v>
       </c>
-      <c r="G18" s="104" t="s">
+      <c r="G18" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="H18" s="104" t="s">
+      <c r="H18" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="104" t="s">
+      <c r="I18" s="86" t="s">
         <v>136</v>
       </c>
-      <c r="J18" s="104" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="105" t="s">
+      <c r="J18" s="86" t="s">
+        <v>277</v>
+      </c>
+      <c r="K18" s="87" t="s">
         <v>134</v>
       </c>
       <c r="L18" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="M18" s="109" t="s">
+      <c r="M18" s="91" t="s">
         <v>139</v>
       </c>
       <c r="O18" s="3"/>
@@ -9660,36 +9591,38 @@
       <c r="AA18" s="2"/>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B19" s="95" t="s">
+      <c r="B19" s="78" t="s">
         <v>146</v>
       </c>
-      <c r="C19" s="96" t="s">
+      <c r="C19" s="79" t="s">
         <v>145</v>
       </c>
       <c r="D19" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="97" t="s">
+      <c r="E19" s="80" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="97" t="s">
-        <v>113</v>
+      <c r="G19" s="80" t="s">
+        <v>81</v>
       </c>
       <c r="H19" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="I19" s="97" t="s">
+      <c r="I19" s="80" t="s">
         <v>118</v>
       </c>
       <c r="J19" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="K19" s="106"/>
-      <c r="L19" s="107"/>
-      <c r="M19" s="110" t="s">
+      <c r="K19" s="88" t="s">
+        <v>81</v>
+      </c>
+      <c r="L19" s="89"/>
+      <c r="M19" s="92" t="s">
         <v>19</v>
       </c>
       <c r="O19" s="3"/>
@@ -9707,36 +9640,36 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B20" s="95" t="s">
+      <c r="B20" s="78" t="s">
         <v>147</v>
       </c>
-      <c r="C20" s="96" t="s">
+      <c r="C20" s="79" t="s">
         <v>148</v>
       </c>
       <c r="D20" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="97" t="s">
+      <c r="E20" s="80" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="97" t="s">
+      <c r="G20" s="80" t="s">
         <v>114</v>
       </c>
       <c r="H20" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="97" t="s">
+      <c r="I20" s="80" t="s">
         <v>119</v>
       </c>
       <c r="J20" s="54"/>
-      <c r="K20" s="106"/>
-      <c r="L20" s="107" t="s">
+      <c r="K20" s="88"/>
+      <c r="L20" s="89" t="s">
         <v>137</v>
       </c>
-      <c r="M20" s="110" t="s">
+      <c r="M20" s="92" t="s">
         <v>74</v>
       </c>
       <c r="O20" s="3"/>
@@ -9752,34 +9685,34 @@
       <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B21" s="95" t="s">
+      <c r="B21" s="78" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="96" t="s">
+      <c r="C21" s="79" t="s">
         <v>149</v>
       </c>
       <c r="D21" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="97" t="s">
+      <c r="E21" s="80" t="s">
         <v>201</v>
       </c>
       <c r="F21" s="54">
         <v>80</v>
       </c>
-      <c r="G21" s="97" t="s">
+      <c r="G21" s="80" t="s">
         <v>73</v>
       </c>
       <c r="H21" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="I21" s="97" t="s">
+      <c r="I21" s="80" t="s">
         <v>61</v>
       </c>
       <c r="J21" s="54"/>
-      <c r="K21" s="106"/>
-      <c r="L21" s="107"/>
-      <c r="M21" s="110"/>
+      <c r="K21" s="88"/>
+      <c r="L21" s="89"/>
+      <c r="M21" s="92"/>
       <c r="O21" s="3"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
@@ -9793,34 +9726,34 @@
       <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B22" s="95" t="s">
+      <c r="B22" s="78" t="s">
         <v>274</v>
       </c>
-      <c r="C22" s="98" t="s">
+      <c r="C22" s="81" t="s">
         <v>275</v>
       </c>
       <c r="D22" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="97" t="s">
+      <c r="E22" s="80" t="s">
         <v>2</v>
       </c>
       <c r="F22" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="97" t="s">
+      <c r="G22" s="80" t="s">
         <v>115</v>
       </c>
       <c r="H22" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="I22" s="97" t="s">
+      <c r="I22" s="80" t="s">
         <v>62</v>
       </c>
       <c r="J22" s="54"/>
-      <c r="K22" s="106"/>
-      <c r="L22" s="107"/>
-      <c r="M22" s="110"/>
+      <c r="K22" s="88"/>
+      <c r="L22" s="89"/>
+      <c r="M22" s="92"/>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
@@ -9833,34 +9766,34 @@
       <c r="AA22" s="2"/>
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B23" s="99" t="s">
+      <c r="B23" s="82" t="s">
         <v>190</v>
       </c>
-      <c r="C23" s="100" t="s">
+      <c r="C23" s="83" t="s">
         <v>203</v>
       </c>
       <c r="D23" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="97" t="s">
+      <c r="E23" s="80" t="s">
         <v>117</v>
       </c>
       <c r="F23" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="97" t="s">
+      <c r="G23" s="80" t="s">
         <v>116</v>
       </c>
       <c r="H23" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="97" t="s">
+      <c r="I23" s="80" t="s">
         <v>63</v>
       </c>
       <c r="J23" s="54"/>
-      <c r="K23" s="106"/>
-      <c r="L23" s="107"/>
-      <c r="M23" s="110"/>
+      <c r="K23" s="88"/>
+      <c r="L23" s="89"/>
+      <c r="M23" s="92"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
@@ -9873,34 +9806,34 @@
       <c r="AA23" s="2"/>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B24" s="95" t="s">
+      <c r="B24" s="78" t="s">
         <v>150</v>
       </c>
-      <c r="C24" s="98" t="s">
+      <c r="C24" s="81" t="s">
         <v>202</v>
       </c>
       <c r="D24" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="E24" s="97" t="s">
+      <c r="E24" s="80" t="s">
         <v>180</v>
       </c>
       <c r="F24" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="G24" s="97" t="s">
+      <c r="G24" s="80" t="s">
         <v>181</v>
       </c>
       <c r="H24" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="I24" s="97" t="s">
+      <c r="I24" s="80" t="s">
         <v>64</v>
       </c>
       <c r="J24" s="54"/>
-      <c r="K24" s="106"/>
-      <c r="L24" s="107"/>
-      <c r="M24" s="110"/>
+      <c r="K24" s="88"/>
+      <c r="L24" s="89"/>
+      <c r="M24" s="92"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
@@ -9913,34 +9846,34 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B25" s="99" t="s">
+      <c r="B25" s="82" t="s">
         <v>190</v>
       </c>
-      <c r="C25" s="100" t="s">
+      <c r="C25" s="83" t="s">
         <v>203</v>
       </c>
       <c r="D25" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="E25" s="97" t="s">
+      <c r="E25" s="80" t="s">
         <v>151</v>
       </c>
       <c r="F25" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="G25" s="97" t="s">
+      <c r="G25" s="80" t="s">
         <v>182</v>
       </c>
       <c r="H25" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="I25" s="97" t="s">
+      <c r="I25" s="80" t="s">
         <v>120</v>
       </c>
       <c r="J25" s="54"/>
-      <c r="K25" s="106"/>
-      <c r="L25" s="107"/>
-      <c r="M25" s="110"/>
+      <c r="K25" s="88"/>
+      <c r="L25" s="89"/>
+      <c r="M25" s="92"/>
       <c r="T25"/>
       <c r="U25"/>
       <c r="V25" s="3"/>
@@ -9949,30 +9882,30 @@
       <c r="Y25"/>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B26" s="101"/>
-      <c r="C26" s="100"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="83"/>
       <c r="D26" s="54" t="s">
         <v>224</v>
       </c>
-      <c r="E26" s="97" t="s">
+      <c r="E26" s="80" t="s">
         <v>225</v>
       </c>
       <c r="F26" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="G26" s="97" t="s">
+      <c r="G26" s="80" t="s">
         <v>183</v>
       </c>
       <c r="H26" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="I26" s="97" t="s">
+      <c r="I26" s="80" t="s">
         <v>65</v>
       </c>
       <c r="J26" s="54"/>
-      <c r="K26" s="106"/>
-      <c r="L26" s="107"/>
-      <c r="M26" s="110"/>
+      <c r="K26" s="88"/>
+      <c r="L26" s="89"/>
+      <c r="M26" s="92"/>
       <c r="R26" s="3"/>
       <c r="S26" s="2"/>
       <c r="T26"/>
@@ -9983,22 +9916,22 @@
       <c r="Y26"/>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B27" s="99"/>
-      <c r="C27" s="100"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="83"/>
       <c r="D27" s="54"/>
-      <c r="E27" s="97"/>
+      <c r="E27" s="80"/>
       <c r="F27" s="54"/>
-      <c r="G27" s="97"/>
+      <c r="G27" s="80"/>
       <c r="H27" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="I27" s="97" t="s">
+      <c r="I27" s="80" t="s">
         <v>121</v>
       </c>
       <c r="J27" s="54"/>
-      <c r="K27" s="106"/>
-      <c r="L27" s="107"/>
-      <c r="M27" s="110"/>
+      <c r="K27" s="88"/>
+      <c r="L27" s="89"/>
+      <c r="M27" s="92"/>
       <c r="R27" s="3"/>
       <c r="S27" s="2"/>
       <c r="T27"/>
@@ -10007,22 +9940,22 @@
       <c r="AA27" s="4"/>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B28" s="101"/>
-      <c r="C28" s="100"/>
+      <c r="B28" s="84"/>
+      <c r="C28" s="83"/>
       <c r="D28" s="54"/>
-      <c r="E28" s="97"/>
+      <c r="E28" s="80"/>
       <c r="F28" s="54"/>
-      <c r="G28" s="97"/>
+      <c r="G28" s="80"/>
       <c r="H28" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="I28" s="97" t="s">
+      <c r="I28" s="80" t="s">
         <v>66</v>
       </c>
       <c r="J28" s="54"/>
-      <c r="K28" s="106"/>
-      <c r="L28" s="107"/>
-      <c r="M28" s="110"/>
+      <c r="K28" s="88"/>
+      <c r="L28" s="89"/>
+      <c r="M28" s="92"/>
       <c r="S28"/>
       <c r="T28"/>
       <c r="U28"/>
@@ -10032,22 +9965,22 @@
       <c r="Y28" s="2"/>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B29" s="99"/>
-      <c r="C29" s="100"/>
+      <c r="B29" s="82"/>
+      <c r="C29" s="83"/>
       <c r="D29" s="54"/>
-      <c r="E29" s="97"/>
+      <c r="E29" s="80"/>
       <c r="F29" s="54"/>
-      <c r="G29" s="97"/>
+      <c r="G29" s="80"/>
       <c r="H29" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="I29" s="97" t="s">
+      <c r="I29" s="80" t="s">
         <v>122</v>
       </c>
       <c r="J29" s="54"/>
-      <c r="K29" s="106"/>
-      <c r="L29" s="107"/>
-      <c r="M29" s="110"/>
+      <c r="K29" s="88"/>
+      <c r="L29" s="89"/>
+      <c r="M29" s="92"/>
       <c r="S29"/>
       <c r="T29"/>
       <c r="U29"/>
@@ -10057,22 +9990,22 @@
       <c r="Y29" s="2"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B30" s="101"/>
-      <c r="C30" s="100"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="83"/>
       <c r="D30" s="54"/>
-      <c r="E30" s="97"/>
+      <c r="E30" s="80"/>
       <c r="F30" s="54"/>
-      <c r="G30" s="97"/>
+      <c r="G30" s="80"/>
       <c r="H30" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="I30" s="97" t="s">
+      <c r="I30" s="80" t="s">
         <v>67</v>
       </c>
       <c r="J30" s="54"/>
-      <c r="K30" s="106"/>
-      <c r="L30" s="107"/>
-      <c r="M30" s="110"/>
+      <c r="K30" s="88"/>
+      <c r="L30" s="89"/>
+      <c r="M30" s="92"/>
       <c r="S30"/>
       <c r="T30"/>
       <c r="U30"/>
@@ -10082,22 +10015,22 @@
       <c r="Y30" s="2"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B31" s="99"/>
-      <c r="C31" s="100"/>
+      <c r="B31" s="82"/>
+      <c r="C31" s="83"/>
       <c r="D31" s="54"/>
-      <c r="E31" s="97"/>
+      <c r="E31" s="80"/>
       <c r="F31" s="54"/>
-      <c r="G31" s="97"/>
+      <c r="G31" s="80"/>
       <c r="H31" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="I31" s="97" t="s">
+      <c r="I31" s="80" t="s">
         <v>123</v>
       </c>
       <c r="J31" s="54"/>
-      <c r="K31" s="106"/>
-      <c r="L31" s="107"/>
-      <c r="M31" s="110"/>
+      <c r="K31" s="88"/>
+      <c r="L31" s="89"/>
+      <c r="M31" s="92"/>
       <c r="S31"/>
       <c r="T31"/>
       <c r="U31"/>
@@ -10107,22 +10040,22 @@
       <c r="Y31" s="2"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B32" s="101"/>
-      <c r="C32" s="100"/>
+      <c r="B32" s="84"/>
+      <c r="C32" s="83"/>
       <c r="D32" s="54"/>
-      <c r="E32" s="97"/>
+      <c r="E32" s="80"/>
       <c r="F32" s="54"/>
-      <c r="G32" s="97"/>
+      <c r="G32" s="80"/>
       <c r="H32" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="I32" s="97" t="s">
+      <c r="I32" s="80" t="s">
         <v>124</v>
       </c>
       <c r="J32" s="54"/>
-      <c r="K32" s="106"/>
-      <c r="L32" s="107"/>
-      <c r="M32" s="110"/>
+      <c r="K32" s="88"/>
+      <c r="L32" s="89"/>
+      <c r="M32" s="92"/>
       <c r="S32"/>
       <c r="T32"/>
       <c r="U32"/>
@@ -10132,22 +10065,22 @@
       <c r="Y32" s="2"/>
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B33" s="99"/>
-      <c r="C33" s="97"/>
+      <c r="B33" s="82"/>
+      <c r="C33" s="80"/>
       <c r="D33" s="54"/>
-      <c r="E33" s="97"/>
+      <c r="E33" s="80"/>
       <c r="F33" s="54"/>
-      <c r="G33" s="97"/>
+      <c r="G33" s="80"/>
       <c r="H33" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="I33" s="97" t="s">
+      <c r="I33" s="80" t="s">
         <v>125</v>
       </c>
       <c r="J33" s="54"/>
-      <c r="K33" s="106"/>
-      <c r="L33" s="107"/>
-      <c r="M33" s="110"/>
+      <c r="K33" s="88"/>
+      <c r="L33" s="89"/>
+      <c r="M33" s="92"/>
       <c r="S33"/>
       <c r="T33"/>
       <c r="U33"/>
@@ -10157,22 +10090,22 @@
       <c r="Y33" s="2"/>
     </row>
     <row r="34" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B34" s="99"/>
-      <c r="C34" s="97"/>
+      <c r="B34" s="82"/>
+      <c r="C34" s="80"/>
       <c r="D34" s="54"/>
-      <c r="E34" s="97"/>
+      <c r="E34" s="80"/>
       <c r="F34" s="54"/>
-      <c r="G34" s="97"/>
+      <c r="G34" s="80"/>
       <c r="H34" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="I34" s="97" t="s">
+      <c r="I34" s="80" t="s">
         <v>126</v>
       </c>
       <c r="J34" s="54"/>
-      <c r="K34" s="106"/>
-      <c r="L34" s="107"/>
-      <c r="M34" s="110"/>
+      <c r="K34" s="88"/>
+      <c r="L34" s="89"/>
+      <c r="M34" s="92"/>
       <c r="S34"/>
       <c r="T34"/>
       <c r="U34"/>
@@ -10182,22 +10115,22 @@
       <c r="Y34" s="2"/>
     </row>
     <row r="35" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B35" s="99"/>
-      <c r="C35" s="97"/>
+      <c r="B35" s="82"/>
+      <c r="C35" s="80"/>
       <c r="D35" s="54"/>
-      <c r="E35" s="97"/>
+      <c r="E35" s="80"/>
       <c r="F35" s="54"/>
-      <c r="G35" s="97"/>
+      <c r="G35" s="80"/>
       <c r="H35" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="I35" s="97" t="s">
+      <c r="I35" s="80" t="s">
         <v>127</v>
       </c>
       <c r="J35" s="54"/>
-      <c r="K35" s="106"/>
-      <c r="L35" s="107"/>
-      <c r="M35" s="110"/>
+      <c r="K35" s="88"/>
+      <c r="L35" s="89"/>
+      <c r="M35" s="92"/>
       <c r="S35"/>
       <c r="T35"/>
       <c r="U35"/>
@@ -10207,44 +10140,44 @@
       <c r="Y35" s="2"/>
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B36" s="99"/>
-      <c r="C36" s="97"/>
+      <c r="B36" s="82"/>
+      <c r="C36" s="80"/>
       <c r="D36" s="54"/>
-      <c r="E36" s="97"/>
+      <c r="E36" s="80"/>
       <c r="F36" s="54"/>
-      <c r="G36" s="97"/>
+      <c r="G36" s="80"/>
       <c r="H36" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="I36" s="97" t="s">
+      <c r="I36" s="80" t="s">
         <v>128</v>
       </c>
       <c r="J36" s="54"/>
-      <c r="K36" s="106"/>
-      <c r="L36" s="107"/>
-      <c r="M36" s="110"/>
+      <c r="K36" s="88"/>
+      <c r="L36" s="89"/>
+      <c r="M36" s="92"/>
       <c r="S36"/>
       <c r="T36"/>
       <c r="U36"/>
       <c r="Y36"/>
     </row>
     <row r="37" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B37" s="99"/>
-      <c r="C37" s="100"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="83"/>
       <c r="D37" s="54"/>
-      <c r="E37" s="97"/>
+      <c r="E37" s="80"/>
       <c r="F37" s="54"/>
-      <c r="G37" s="97"/>
+      <c r="G37" s="80"/>
       <c r="H37" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="I37" s="97" t="s">
+      <c r="I37" s="80" t="s">
         <v>129</v>
       </c>
       <c r="J37" s="54"/>
-      <c r="K37" s="106"/>
-      <c r="L37" s="107"/>
-      <c r="M37" s="110"/>
+      <c r="K37" s="88"/>
+      <c r="L37" s="89"/>
+      <c r="M37" s="92"/>
       <c r="S37"/>
       <c r="T37"/>
       <c r="U37"/>
@@ -10254,22 +10187,22 @@
       <c r="Y37"/>
     </row>
     <row r="38" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B38" s="101"/>
-      <c r="C38" s="100"/>
+      <c r="B38" s="84"/>
+      <c r="C38" s="83"/>
       <c r="D38" s="54"/>
-      <c r="E38" s="97"/>
+      <c r="E38" s="80"/>
       <c r="F38" s="54"/>
-      <c r="G38" s="97"/>
+      <c r="G38" s="80"/>
       <c r="H38" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="I38" s="97" t="s">
+      <c r="I38" s="80" t="s">
         <v>130</v>
       </c>
       <c r="J38" s="54"/>
-      <c r="K38" s="106"/>
-      <c r="L38" s="107"/>
-      <c r="M38" s="110"/>
+      <c r="K38" s="88"/>
+      <c r="L38" s="89"/>
+      <c r="M38" s="92"/>
       <c r="R38" s="3"/>
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
@@ -10280,479 +10213,473 @@
       <c r="Y38"/>
     </row>
     <row r="39" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B39" s="99"/>
-      <c r="C39" s="100"/>
+      <c r="B39" s="82"/>
+      <c r="C39" s="83"/>
       <c r="D39" s="54"/>
-      <c r="E39" s="97"/>
+      <c r="E39" s="80"/>
       <c r="F39" s="54"/>
-      <c r="G39" s="97"/>
+      <c r="G39" s="80"/>
       <c r="H39" s="54"/>
-      <c r="I39" s="97"/>
+      <c r="I39" s="80"/>
       <c r="J39" s="54"/>
-      <c r="K39" s="106"/>
-      <c r="L39" s="107"/>
-      <c r="M39" s="110"/>
+      <c r="K39" s="88"/>
+      <c r="L39" s="89"/>
+      <c r="M39" s="92"/>
       <c r="X39"/>
       <c r="Y39"/>
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B40" s="101"/>
-      <c r="C40" s="100"/>
+      <c r="B40" s="84"/>
+      <c r="C40" s="83"/>
       <c r="D40" s="54"/>
-      <c r="E40" s="97"/>
+      <c r="E40" s="80"/>
       <c r="F40" s="54"/>
-      <c r="G40" s="97"/>
+      <c r="G40" s="80"/>
       <c r="H40" s="54"/>
-      <c r="I40" s="97"/>
+      <c r="I40" s="80"/>
       <c r="J40" s="54"/>
-      <c r="K40" s="106"/>
-      <c r="L40" s="107"/>
-      <c r="M40" s="110"/>
+      <c r="K40" s="88"/>
+      <c r="L40" s="89"/>
+      <c r="M40" s="92"/>
       <c r="X40"/>
       <c r="Y40"/>
     </row>
     <row r="41" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="B41" s="99"/>
-      <c r="C41" s="100"/>
+      <c r="B41" s="82"/>
+      <c r="C41" s="83"/>
       <c r="D41" s="54"/>
-      <c r="E41" s="97"/>
+      <c r="E41" s="80"/>
       <c r="F41" s="54"/>
-      <c r="G41" s="97"/>
+      <c r="G41" s="80"/>
       <c r="H41" s="54"/>
-      <c r="I41" s="97"/>
+      <c r="I41" s="80"/>
       <c r="J41" s="54"/>
-      <c r="K41" s="106"/>
-      <c r="L41" s="107"/>
-      <c r="M41" s="110"/>
+      <c r="K41" s="88"/>
+      <c r="L41" s="89"/>
+      <c r="M41" s="92"/>
       <c r="X41"/>
       <c r="Y41"/>
     </row>
     <row r="42" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="101"/>
-      <c r="C42" s="100"/>
+      <c r="B42" s="84"/>
+      <c r="C42" s="83"/>
       <c r="D42" s="54"/>
-      <c r="E42" s="97"/>
+      <c r="E42" s="80"/>
       <c r="F42" s="54"/>
-      <c r="G42" s="97"/>
+      <c r="G42" s="80"/>
       <c r="H42" s="54"/>
-      <c r="I42" s="97"/>
+      <c r="I42" s="80"/>
       <c r="J42" s="54"/>
-      <c r="K42" s="106"/>
-      <c r="L42" s="107"/>
-      <c r="M42" s="110"/>
+      <c r="K42" s="88"/>
+      <c r="L42" s="89"/>
+      <c r="M42" s="92"/>
       <c r="X42"/>
       <c r="Y42"/>
     </row>
     <row r="43" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="99"/>
-      <c r="C43" s="100"/>
+      <c r="B43" s="82"/>
+      <c r="C43" s="83"/>
       <c r="D43" s="54"/>
-      <c r="E43" s="97"/>
+      <c r="E43" s="80"/>
       <c r="F43" s="54"/>
-      <c r="G43" s="97"/>
+      <c r="G43" s="80"/>
       <c r="H43" s="54"/>
-      <c r="I43" s="97"/>
+      <c r="I43" s="80"/>
       <c r="J43" s="54"/>
-      <c r="K43" s="106"/>
-      <c r="L43" s="107"/>
-      <c r="M43" s="110"/>
+      <c r="K43" s="88"/>
+      <c r="L43" s="89"/>
+      <c r="M43" s="92"/>
       <c r="X43"/>
       <c r="Y43"/>
     </row>
     <row r="44" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="101"/>
-      <c r="C44" s="100"/>
+      <c r="B44" s="84"/>
+      <c r="C44" s="83"/>
       <c r="D44" s="54"/>
-      <c r="E44" s="97"/>
+      <c r="E44" s="80"/>
       <c r="F44" s="54"/>
-      <c r="G44" s="97"/>
+      <c r="G44" s="80"/>
       <c r="H44" s="54"/>
-      <c r="I44" s="97"/>
+      <c r="I44" s="80"/>
       <c r="J44" s="54"/>
-      <c r="K44" s="106"/>
-      <c r="L44" s="107"/>
-      <c r="M44" s="110"/>
+      <c r="K44" s="88"/>
+      <c r="L44" s="89"/>
+      <c r="M44" s="92"/>
       <c r="X44"/>
       <c r="Y44"/>
     </row>
     <row r="45" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="99"/>
-      <c r="C45" s="100"/>
+      <c r="B45" s="82"/>
+      <c r="C45" s="83"/>
       <c r="D45" s="54"/>
-      <c r="E45" s="97"/>
+      <c r="E45" s="80"/>
       <c r="F45" s="54"/>
-      <c r="G45" s="97"/>
+      <c r="G45" s="80"/>
       <c r="H45" s="54"/>
-      <c r="I45" s="97"/>
+      <c r="I45" s="80"/>
       <c r="J45" s="54"/>
-      <c r="K45" s="106"/>
-      <c r="L45" s="107"/>
-      <c r="M45" s="110"/>
+      <c r="K45" s="88"/>
+      <c r="L45" s="89"/>
+      <c r="M45" s="92"/>
       <c r="X45"/>
       <c r="Y45"/>
     </row>
     <row r="46" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="101"/>
-      <c r="C46" s="100"/>
+      <c r="B46" s="84"/>
+      <c r="C46" s="83"/>
       <c r="D46" s="54"/>
-      <c r="E46" s="97"/>
+      <c r="E46" s="80"/>
       <c r="F46" s="54"/>
-      <c r="G46" s="97"/>
+      <c r="G46" s="80"/>
       <c r="H46" s="54"/>
-      <c r="I46" s="97"/>
+      <c r="I46" s="80"/>
       <c r="J46" s="54"/>
-      <c r="K46" s="106"/>
-      <c r="L46" s="107"/>
-      <c r="M46" s="110"/>
+      <c r="K46" s="88"/>
+      <c r="L46" s="89"/>
+      <c r="M46" s="92"/>
       <c r="X46"/>
       <c r="Y46"/>
     </row>
     <row r="47" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="99"/>
-      <c r="C47" s="100"/>
+      <c r="B47" s="82"/>
+      <c r="C47" s="83"/>
       <c r="D47" s="54"/>
-      <c r="E47" s="97"/>
+      <c r="E47" s="80"/>
       <c r="F47" s="54"/>
-      <c r="G47" s="97"/>
+      <c r="G47" s="80"/>
       <c r="H47" s="54"/>
-      <c r="I47" s="97"/>
+      <c r="I47" s="80"/>
       <c r="J47" s="54"/>
-      <c r="K47" s="106"/>
-      <c r="L47" s="107"/>
-      <c r="M47" s="110"/>
+      <c r="K47" s="88"/>
+      <c r="L47" s="89"/>
+      <c r="M47" s="92"/>
       <c r="X47"/>
       <c r="Y47"/>
     </row>
     <row r="48" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="101"/>
-      <c r="C48" s="100"/>
+      <c r="B48" s="84"/>
+      <c r="C48" s="83"/>
       <c r="D48" s="54"/>
-      <c r="E48" s="97"/>
+      <c r="E48" s="80"/>
       <c r="F48" s="54"/>
-      <c r="G48" s="97"/>
+      <c r="G48" s="80"/>
       <c r="H48" s="54"/>
-      <c r="I48" s="97"/>
+      <c r="I48" s="80"/>
       <c r="J48" s="54"/>
-      <c r="K48" s="106"/>
-      <c r="L48" s="107"/>
-      <c r="M48" s="110"/>
+      <c r="K48" s="88"/>
+      <c r="L48" s="89"/>
+      <c r="M48" s="92"/>
       <c r="X48"/>
       <c r="Y48"/>
     </row>
     <row r="49" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="99"/>
-      <c r="C49" s="100"/>
+      <c r="B49" s="82"/>
+      <c r="C49" s="83"/>
       <c r="D49" s="54"/>
-      <c r="E49" s="97"/>
+      <c r="E49" s="80"/>
       <c r="F49" s="54"/>
-      <c r="G49" s="97"/>
+      <c r="G49" s="80"/>
       <c r="H49" s="54"/>
-      <c r="I49" s="97"/>
+      <c r="I49" s="80"/>
       <c r="J49" s="54"/>
-      <c r="K49" s="106"/>
-      <c r="L49" s="107"/>
-      <c r="M49" s="110"/>
+      <c r="K49" s="88"/>
+      <c r="L49" s="89"/>
+      <c r="M49" s="92"/>
       <c r="X49"/>
       <c r="Y49"/>
     </row>
     <row r="50" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="101"/>
-      <c r="C50" s="100"/>
+      <c r="B50" s="84"/>
+      <c r="C50" s="83"/>
       <c r="D50" s="54"/>
-      <c r="E50" s="97"/>
+      <c r="E50" s="80"/>
       <c r="F50" s="54"/>
-      <c r="G50" s="97"/>
+      <c r="G50" s="80"/>
       <c r="H50" s="54"/>
-      <c r="I50" s="97"/>
+      <c r="I50" s="80"/>
       <c r="J50" s="54"/>
-      <c r="K50" s="106"/>
-      <c r="L50" s="107"/>
-      <c r="M50" s="110"/>
+      <c r="K50" s="88"/>
+      <c r="L50" s="89"/>
+      <c r="M50" s="92"/>
       <c r="X50"/>
       <c r="Y50"/>
     </row>
     <row r="51" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="99"/>
-      <c r="C51" s="100"/>
+      <c r="B51" s="82"/>
+      <c r="C51" s="83"/>
       <c r="D51" s="54"/>
-      <c r="E51" s="97"/>
+      <c r="E51" s="80"/>
       <c r="F51" s="54"/>
-      <c r="G51" s="97"/>
+      <c r="G51" s="80"/>
       <c r="H51" s="54"/>
-      <c r="I51" s="97"/>
+      <c r="I51" s="80"/>
       <c r="J51" s="54"/>
-      <c r="K51" s="106"/>
-      <c r="L51" s="107"/>
-      <c r="M51" s="110"/>
+      <c r="K51" s="88"/>
+      <c r="L51" s="89"/>
+      <c r="M51" s="92"/>
       <c r="X51"/>
       <c r="Y51"/>
     </row>
     <row r="52" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="99"/>
-      <c r="C52" s="100"/>
+      <c r="B52" s="82"/>
+      <c r="C52" s="83"/>
       <c r="D52" s="54"/>
-      <c r="E52" s="97"/>
+      <c r="E52" s="80"/>
       <c r="F52" s="54"/>
-      <c r="G52" s="97"/>
+      <c r="G52" s="80"/>
       <c r="H52" s="54"/>
-      <c r="I52" s="97"/>
+      <c r="I52" s="80"/>
       <c r="J52" s="54"/>
-      <c r="K52" s="106"/>
-      <c r="L52" s="107"/>
-      <c r="M52" s="110"/>
+      <c r="K52" s="88"/>
+      <c r="L52" s="89"/>
+      <c r="M52" s="92"/>
       <c r="X52"/>
       <c r="Y52"/>
     </row>
     <row r="53" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="101"/>
-      <c r="C53" s="100"/>
+      <c r="B53" s="84"/>
+      <c r="C53" s="83"/>
       <c r="D53" s="54"/>
-      <c r="E53" s="97"/>
+      <c r="E53" s="80"/>
       <c r="F53" s="54"/>
-      <c r="G53" s="97"/>
+      <c r="G53" s="80"/>
       <c r="H53" s="54"/>
-      <c r="I53" s="97"/>
+      <c r="I53" s="80"/>
       <c r="J53" s="54"/>
-      <c r="K53" s="106"/>
-      <c r="L53" s="107"/>
-      <c r="M53" s="110"/>
+      <c r="K53" s="88"/>
+      <c r="L53" s="89"/>
+      <c r="M53" s="92"/>
       <c r="X53"/>
       <c r="Y53"/>
     </row>
     <row r="54" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="99"/>
-      <c r="C54" s="100"/>
+      <c r="B54" s="82"/>
+      <c r="C54" s="83"/>
       <c r="D54" s="54"/>
-      <c r="E54" s="97"/>
+      <c r="E54" s="80"/>
       <c r="F54" s="54"/>
-      <c r="G54" s="97"/>
+      <c r="G54" s="80"/>
       <c r="H54" s="54"/>
-      <c r="I54" s="97"/>
+      <c r="I54" s="80"/>
       <c r="J54" s="54"/>
-      <c r="K54" s="106"/>
-      <c r="L54" s="107"/>
-      <c r="M54" s="110"/>
+      <c r="K54" s="88"/>
+      <c r="L54" s="89"/>
+      <c r="M54" s="92"/>
       <c r="X54"/>
       <c r="Y54"/>
     </row>
     <row r="55" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="101"/>
-      <c r="C55" s="100"/>
+      <c r="B55" s="84"/>
+      <c r="C55" s="83"/>
       <c r="D55" s="54"/>
-      <c r="E55" s="97"/>
+      <c r="E55" s="80"/>
       <c r="F55" s="54"/>
-      <c r="G55" s="97"/>
+      <c r="G55" s="80"/>
       <c r="H55" s="54"/>
-      <c r="I55" s="97"/>
+      <c r="I55" s="80"/>
       <c r="J55" s="54"/>
-      <c r="K55" s="106"/>
-      <c r="L55" s="107"/>
-      <c r="M55" s="110"/>
+      <c r="K55" s="88"/>
+      <c r="L55" s="89"/>
+      <c r="M55" s="92"/>
       <c r="X55"/>
       <c r="Y55"/>
     </row>
     <row r="56" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="101"/>
-      <c r="C56" s="100"/>
+      <c r="B56" s="84"/>
+      <c r="C56" s="83"/>
       <c r="D56" s="54"/>
-      <c r="E56" s="97"/>
+      <c r="E56" s="80"/>
       <c r="F56" s="54"/>
-      <c r="G56" s="97"/>
+      <c r="G56" s="80"/>
       <c r="H56" s="54"/>
-      <c r="I56" s="97"/>
+      <c r="I56" s="80"/>
       <c r="J56" s="54"/>
-      <c r="K56" s="106"/>
-      <c r="L56" s="107"/>
-      <c r="M56" s="110"/>
+      <c r="K56" s="88"/>
+      <c r="L56" s="89"/>
+      <c r="M56" s="92"/>
       <c r="X56"/>
       <c r="Y56"/>
     </row>
     <row r="57" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="99"/>
-      <c r="C57" s="100"/>
+      <c r="B57" s="82"/>
+      <c r="C57" s="83"/>
       <c r="D57" s="54"/>
-      <c r="E57" s="97"/>
+      <c r="E57" s="80"/>
       <c r="F57" s="54"/>
-      <c r="G57" s="97"/>
+      <c r="G57" s="80"/>
       <c r="H57" s="54"/>
-      <c r="I57" s="97"/>
+      <c r="I57" s="80"/>
       <c r="J57" s="54"/>
-      <c r="K57" s="106"/>
-      <c r="L57" s="107"/>
-      <c r="M57" s="110"/>
+      <c r="K57" s="88"/>
+      <c r="L57" s="89"/>
+      <c r="M57" s="92"/>
       <c r="X57"/>
       <c r="Y57"/>
     </row>
     <row r="58" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="101"/>
-      <c r="C58" s="100"/>
+      <c r="B58" s="84"/>
+      <c r="C58" s="83"/>
       <c r="D58" s="54"/>
-      <c r="E58" s="97"/>
+      <c r="E58" s="80"/>
       <c r="F58" s="54"/>
-      <c r="G58" s="97"/>
+      <c r="G58" s="80"/>
       <c r="H58" s="54"/>
-      <c r="I58" s="97"/>
+      <c r="I58" s="80"/>
       <c r="J58" s="54"/>
-      <c r="K58" s="106"/>
-      <c r="L58" s="107"/>
-      <c r="M58" s="110"/>
+      <c r="K58" s="88"/>
+      <c r="L58" s="89"/>
+      <c r="M58" s="92"/>
       <c r="X58"/>
       <c r="Y58"/>
     </row>
     <row r="59" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="99"/>
-      <c r="C59" s="100"/>
+      <c r="B59" s="82"/>
+      <c r="C59" s="83"/>
       <c r="D59" s="54"/>
-      <c r="E59" s="97"/>
+      <c r="E59" s="80"/>
       <c r="F59" s="54"/>
-      <c r="G59" s="97"/>
+      <c r="G59" s="80"/>
       <c r="H59" s="54"/>
-      <c r="I59" s="97"/>
+      <c r="I59" s="80"/>
       <c r="J59" s="54"/>
-      <c r="K59" s="106"/>
-      <c r="L59" s="107"/>
-      <c r="M59" s="110"/>
+      <c r="K59" s="88"/>
+      <c r="L59" s="89"/>
+      <c r="M59" s="92"/>
       <c r="X59"/>
       <c r="Y59"/>
     </row>
     <row r="60" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="101"/>
-      <c r="C60" s="100"/>
+      <c r="B60" s="84"/>
+      <c r="C60" s="83"/>
       <c r="D60" s="54"/>
-      <c r="E60" s="97"/>
+      <c r="E60" s="80"/>
       <c r="F60" s="54"/>
-      <c r="G60" s="97"/>
+      <c r="G60" s="80"/>
       <c r="H60" s="54"/>
-      <c r="I60" s="97"/>
+      <c r="I60" s="80"/>
       <c r="J60" s="54"/>
-      <c r="K60" s="106"/>
-      <c r="L60" s="107"/>
-      <c r="M60" s="110"/>
+      <c r="K60" s="88"/>
+      <c r="L60" s="89"/>
+      <c r="M60" s="92"/>
       <c r="X60"/>
       <c r="Y60"/>
     </row>
     <row r="61" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="99"/>
-      <c r="C61" s="100"/>
+      <c r="B61" s="82"/>
+      <c r="C61" s="83"/>
       <c r="D61" s="54"/>
-      <c r="E61" s="97"/>
+      <c r="E61" s="80"/>
       <c r="F61" s="54"/>
-      <c r="G61" s="97"/>
+      <c r="G61" s="80"/>
       <c r="H61" s="54"/>
-      <c r="I61" s="97"/>
+      <c r="I61" s="80"/>
       <c r="J61" s="54"/>
-      <c r="K61" s="106"/>
-      <c r="L61" s="107"/>
-      <c r="M61" s="110"/>
+      <c r="K61" s="88"/>
+      <c r="L61" s="89"/>
+      <c r="M61" s="92"/>
     </row>
     <row r="62" spans="2:25" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="99"/>
-      <c r="C62" s="97"/>
+      <c r="B62" s="82"/>
+      <c r="C62" s="80"/>
       <c r="D62" s="54"/>
-      <c r="E62" s="97"/>
+      <c r="E62" s="80"/>
       <c r="F62" s="54"/>
-      <c r="G62" s="97"/>
+      <c r="G62" s="80"/>
       <c r="H62" s="54"/>
-      <c r="I62" s="97"/>
+      <c r="I62" s="80"/>
       <c r="J62" s="54"/>
-      <c r="K62" s="106"/>
-      <c r="L62" s="108"/>
-      <c r="M62" s="111"/>
-    </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B70" s="8" t="s">
+      <c r="K62" s="88"/>
+      <c r="L62" s="90"/>
+      <c r="M62" s="93"/>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B69" s="8" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B71" s="95" t="s">
+    <row r="70" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B70" s="78" t="s">
         <v>146</v>
       </c>
-      <c r="C71" s="96"/>
+      <c r="C70" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="D70" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="80" t="s">
+        <v>1</v>
+      </c>
+      <c r="F70" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="G70" s="80" t="s">
+        <v>114</v>
+      </c>
+      <c r="H70" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="I70" s="80" t="s">
+        <v>118</v>
+      </c>
+      <c r="J70" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="K70" s="88" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B71" s="78" t="s">
+        <v>147</v>
+      </c>
+      <c r="C71" s="79" t="s">
+        <v>148</v>
+      </c>
       <c r="D71" s="54" t="s">
-        <v>11</v>
-      </c>
-      <c r="E71" s="97"/>
-      <c r="F71" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="G71" s="97"/>
+        <v>12</v>
+      </c>
+      <c r="E71" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="F71" s="54">
+        <v>80</v>
+      </c>
+      <c r="G71" s="80" t="s">
+        <v>73</v>
+      </c>
       <c r="H71" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="I71" s="97"/>
-      <c r="J71" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="K71" s="97"/>
-      <c r="L71" s="102"/>
-      <c r="M71" s="112"/>
-    </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B72" s="95" t="s">
-        <v>147</v>
-      </c>
-      <c r="C72" s="96"/>
+        <v>38</v>
+      </c>
+      <c r="I71" s="80" t="s">
+        <v>119</v>
+      </c>
+      <c r="J71" s="54"/>
+      <c r="K71" s="88"/>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B72" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="C72" s="79" t="s">
+        <v>149</v>
+      </c>
       <c r="D72" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="E72" s="97"/>
-      <c r="F72" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="G72" s="97"/>
+        <v>13</v>
+      </c>
+      <c r="E72" s="80" t="s">
+        <v>201</v>
+      </c>
+      <c r="F72" s="54"/>
+      <c r="G72" s="80"/>
       <c r="H72" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="I72" s="97"/>
+        <v>40</v>
+      </c>
+      <c r="I72" s="80" t="s">
+        <v>61</v>
+      </c>
       <c r="J72" s="54"/>
-      <c r="K72" s="97"/>
-      <c r="L72" s="102"/>
-      <c r="M72" s="112"/>
-    </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B73" s="95" t="s">
-        <v>144</v>
-      </c>
-      <c r="C73" s="96"/>
-      <c r="D73" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="E73" s="97"/>
-      <c r="F73" s="54">
-        <v>80</v>
-      </c>
-      <c r="G73" s="97"/>
-      <c r="H73" s="54" t="s">
-        <v>40</v>
-      </c>
-      <c r="I73" s="97"/>
-      <c r="J73" s="54"/>
-      <c r="K73" s="97"/>
-      <c r="L73" s="102"/>
-      <c r="M73" s="112"/>
-    </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B74" s="95" t="s">
-        <v>274</v>
-      </c>
-      <c r="C74" s="98"/>
-      <c r="D74" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="E74" s="97"/>
-      <c r="F74" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="G74" s="97"/>
-      <c r="H74" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="I74" s="97"/>
-      <c r="J74" s="54"/>
-      <c r="K74" s="97"/>
-      <c r="L74" s="102"/>
-      <c r="M74" s="112"/>
+      <c r="K72" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -10762,7 +10689,7 @@
     <mergeCell ref="D10:J10"/>
     <mergeCell ref="K10:L10"/>
   </mergeCells>
-  <dataValidations count="7">
+  <dataValidations disablePrompts="1" count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{AD0A9F7F-E76F-44A0-A111-1BBD2BB9AB2C}">
       <formula1>$B$19:$B$61</formula1>
     </dataValidation>
@@ -10834,11 +10761,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="99" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
       <c r="D1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -10937,7 +10864,7 @@
       <c r="J7" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="K7" s="86" t="str">
+      <c r="K7" s="77" t="str">
         <f>VLOOKUP($K$6,Tabela16624[],2,0)</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -10961,20 +10888,20 @@
         <f>_xlfn.CONCAT(C6:K6)</f>
         <v>NN001-N00-080-001</v>
       </c>
-      <c r="D9" s="119" t="str">
+      <c r="D9" s="100" t="str">
         <f>_xlfn.CONCAT(C7:L7)</f>
         <v xml:space="preserve">Nitonakr. Okr.  A2   M8  </v>
       </c>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="120"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="121"/>
-      <c r="K9" s="124" t="s">
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="105" t="s">
         <v>186</v>
       </c>
-      <c r="L9" s="125"/>
+      <c r="L9" s="106"/>
       <c r="N9" s="4">
         <f>LEN(D9)</f>
         <v>25</v>
@@ -10991,20 +10918,20 @@
         <f>_xlfn.CONCAT(C6:M6)</f>
         <v>NN001-N00-080-001-00</v>
       </c>
-      <c r="D10" s="119" t="str">
+      <c r="D10" s="100" t="str">
         <f>_xlfn.CONCAT(C7:M7)</f>
         <v xml:space="preserve">Nitonakr. Okr.  A2   M8  </v>
       </c>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="120"/>
-      <c r="I10" s="120"/>
-      <c r="J10" s="121"/>
-      <c r="K10" s="122" t="s">
+      <c r="E10" s="101"/>
+      <c r="F10" s="101"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="101"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="103" t="s">
         <v>185</v>
       </c>
-      <c r="L10" s="123"/>
+      <c r="L10" s="104"/>
       <c r="N10" s="4">
         <f>LEN(D10)</f>
         <v>25</v>

</xml_diff>